<commit_message>
all analyzers and output images added
</commit_message>
<xml_diff>
--- a/data/ssym_downsampled_stabilizing.xlsx
+++ b/data/ssym_downsampled_stabilizing.xlsx
@@ -542,7 +542,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2lzm</t>
+          <t>1amq</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -551,35 +551,35 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>164</v>
+        <v>396</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>T157L</t>
+          <t>C191W</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>THR</t>
+          <t>CYS</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>LEU</t>
+          <t>TRP</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.7</v>
+        <v>3.9</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1l11</t>
+          <t>1qit</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -591,7 +591,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1l63</t>
+          <t>1amq</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -600,35 +600,35 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>162</v>
+        <v>396</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>F153A</t>
+          <t>C191Y</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>PHE</t>
+          <t>CYS</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>TYR</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>3.8</v>
+        <v>2.3</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1l85</t>
+          <t>1qir</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1ihb</t>
+          <t>1bni</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -649,35 +649,35 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F82Q</t>
+          <t>L89V</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>PHE</t>
+          <t>LEU</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>GLN</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1mx4</t>
+          <t>1bse</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -689,7 +689,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2rn2</t>
+          <t>1bni</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -698,16 +698,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G77A</t>
+          <t>T26A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>GLY</t>
+          <t>THR</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -716,17 +716,17 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9</v>
+        <v>1.7</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1gob</t>
+          <t>1bns</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1iob</t>
+          <t>1bni</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -747,35 +747,35 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>T9G</t>
+          <t>I88V</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>THR</t>
+          <t>ILE</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>GLY</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1hib</t>
+          <t>1bsc</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -836,7 +836,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1lz1</t>
+          <t>1ey0</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -845,35 +845,35 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>D91P</t>
+          <t>I72L</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ASP</t>
+          <t>ILE</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>PRO</t>
+          <t>LEU</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1lhk</t>
+          <t>2f0i</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -885,7 +885,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4lyz</t>
+          <t>1ey0</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -894,35 +894,35 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>I58M</t>
+          <t>T120V</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ILE</t>
+          <t>THR</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MET</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>1ir8</t>
+          <t>2eyp</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -934,7 +934,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1oh0</t>
+          <t>1ey0</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -943,35 +943,35 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Y57F</t>
+          <t>T82S</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>TYR</t>
+          <t>THR</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PHE</t>
+          <t>SER</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1dmm</t>
+          <t>2eyl</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -983,7 +983,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1bni</t>
+          <t>1ey0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -992,35 +992,35 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>L89V</t>
+          <t>T41S</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LEU</t>
+          <t>THR</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>SER</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5</v>
+        <v>1.1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1bse</t>
+          <t>2ey5</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1032,7 +1032,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1vqb</t>
+          <t>1ihb</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1041,35 +1041,35 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>V35I</t>
+          <t>F82Q</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>PHE</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ILE</t>
+          <t>GLN</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>1vqj</t>
+          <t>1mx4</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1081,7 +1081,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5pti</t>
+          <t>1ihb</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1090,35 +1090,35 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Y23A</t>
+          <t>F92N</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>TYR</t>
+          <t>PHE</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>ASN</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>5.9</v>
+        <v>1.1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1bpt</t>
+          <t>1mx6</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1130,7 +1130,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2lzm</t>
+          <t>1iob</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1139,35 +1139,35 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>K147E</t>
+          <t>T9G</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LYS</t>
+          <t>THR</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>GLU</t>
+          <t>GLY</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7</v>
+        <v>2.6</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1l46</t>
+          <t>1hib</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1192,12 +1192,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>V111A</t>
+          <t>F153A</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>PHE</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1206,17 +1206,17 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>235l</t>
+          <t>1l85</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1ihb</t>
+          <t>1l63</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1237,35 +1237,35 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>F92N</t>
+          <t>V111A</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>PHE</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ASN</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1mx6</t>
+          <t>235l</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1277,7 +1277,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2rn2</t>
+          <t>1l63</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1286,47 +1286,47 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>A52F</t>
+          <t>I27A</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>ILE</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>ALA</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>PHE</t>
-        </is>
-      </c>
       <c r="G18" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0.5</v>
+        <v>3.1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>3aa5</t>
+          <t>240l</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1ey0</t>
+          <t>1l63</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1335,11 +1335,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>I72L</t>
+          <t>I27M</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1349,21 +1349,21 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>LEU</t>
+          <t>MET</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2</v>
+        <v>3.1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2f0i</t>
+          <t>1d2w</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1388,31 +1388,31 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>I106A</t>
+          <t>D91P</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>ILE</t>
+          <t>ASP</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>PRO</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2hea</t>
+          <t>1lhk</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1424,7 +1424,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4lyz</t>
+          <t>1lz1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1433,16 +1433,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>S91A</t>
+          <t>I106A</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>SER</t>
+          <t>ILE</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1451,17 +1451,17 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1lsn</t>
+          <t>2hea</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1473,7 +1473,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1bni</t>
+          <t>1lz1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1482,35 +1482,35 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>T26A</t>
+          <t>V74G</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>THR</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>GLY</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>1.7</v>
+        <v>0.1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1bns</t>
+          <t>1gb5</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1vqb</t>
+          <t>1lz1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1531,11 +1531,11 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>I47L</t>
+          <t>I23V</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1545,11 +1545,11 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>LEU</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1vqg</t>
+          <t>1yan</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1571,7 +1571,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5pti</t>
+          <t>1lz1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1580,35 +1580,35 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>N43G</t>
+          <t>V2Y</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ASN</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>GLY</t>
+          <t>TYR</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>5.7</v>
+        <v>0.4</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1nag</t>
+          <t>1gf9</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1620,7 +1620,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1amq</t>
+          <t>1oh0</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1629,35 +1629,35 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>396</v>
+        <v>125</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>C191W</t>
+          <t>Y57F</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CYS</t>
+          <t>TYR</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>TRP</t>
+          <t>PHE</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>191</v>
+        <v>57</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>3.9</v>
+        <v>1.2</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>1qit</t>
+          <t>1dmm</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1669,7 +1669,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2lzm</t>
+          <t>1vqb</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1678,35 +1678,35 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>164</v>
+        <v>86</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>R96E</t>
+          <t>V35I</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ARG</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>GLU</t>
+          <t>ILE</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>2.5</v>
+        <v>0.6</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>3c8s</t>
+          <t>1vqj</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1l63</t>
+          <t>1vqb</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1727,11 +1727,11 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>I27A</t>
+          <t>I47L</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1741,21 +1741,21 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>LEU</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>3.1</v>
+        <v>0.4</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>240l</t>
+          <t>1vqg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -1767,7 +1767,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1ey0</t>
+          <t>2lzm</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1776,11 +1776,11 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>T120V</t>
+          <t>T157L</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1790,21 +1790,21 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>LEU</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2eyp</t>
+          <t>1l11</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -1816,7 +1816,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1lz1</t>
+          <t>2lzm</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1825,35 +1825,35 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>V74G</t>
+          <t>K147E</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>GLY</t>
+          <t>GLU</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1gb5</t>
+          <t>1l46</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -1865,7 +1865,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4lyz</t>
+          <t>2lzm</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1874,35 +1874,35 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>M12L</t>
+          <t>R96E</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>MET</t>
+          <t>ARG</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>LEU</t>
+          <t>GLU</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0.4</v>
+        <v>2.5</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>1iot</t>
+          <t>3c8s</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -1914,7 +1914,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1bni</t>
+          <t>2lzm</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1923,35 +1923,35 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>I88V</t>
+          <t>V131S</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ILE</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>SER</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>1.6</v>
+        <v>0.1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>1bsc</t>
+          <t>1dye</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -1963,7 +1963,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1l63</t>
+          <t>2rn2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1972,35 +1972,35 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>I27M</t>
+          <t>G77A</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ILE</t>
+          <t>GLY</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>MET</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>3.1</v>
+        <v>0.9</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>1d2w</t>
+          <t>1gob</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2012,7 +2012,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1ey0</t>
+          <t>2rn2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2021,47 +2021,47 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>T82S</t>
+          <t>A52F</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>THR</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>SER</t>
+          <t>PHE</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2eyl</t>
+          <t>3aa5</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1lz1</t>
+          <t>4lyz</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2070,11 +2070,11 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>I23V</t>
+          <t>I58M</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2084,21 +2084,21 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>MET</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1yan</t>
+          <t>1ir8</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2123,12 +2123,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>G67A</t>
+          <t>S91A</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>GLY</t>
+          <t>SER</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2137,17 +2137,17 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>1flu</t>
+          <t>1lsn</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2159,7 +2159,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5pti</t>
+          <t>4lyz</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2168,35 +2168,35 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>F45A</t>
+          <t>M12L</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>PHE</t>
+          <t>MET</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>LEU</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>6.9</v>
+        <v>0.4</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>1fan</t>
+          <t>1iot</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2208,7 +2208,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1amq</t>
+          <t>4lyz</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2217,35 +2217,35 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>396</v>
+        <v>129</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>C191Y</t>
+          <t>G67A</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>CYS</t>
+          <t>GLY</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>TYR</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>191</v>
+        <v>67</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>2.3</v>
+        <v>0.5</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>1qir</t>
+          <t>1flu</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2257,7 +2257,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2lzm</t>
+          <t>4lyz</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2266,35 +2266,35 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>V131S</t>
+          <t>G117A</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>GLY</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>SER</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>1dye</t>
+          <t>1flq</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2306,7 +2306,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1ey0</t>
+          <t>5pti</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2315,35 +2315,35 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>T41S</t>
+          <t>Y23A</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>THR</t>
+          <t>TYR</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>SER</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="H39" t="b">
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>1.1</v>
+        <v>5.9</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2ey5</t>
+          <t>1bpt</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -2355,7 +2355,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1lz1</t>
+          <t>5pti</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2364,35 +2364,35 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>V2Y</t>
+          <t>N43G</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>ASN</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>TYR</t>
+          <t>GLY</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.4</v>
+        <v>5.7</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>1gf9</t>
+          <t>1nag</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -2404,7 +2404,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4lyz</t>
+          <t>5pti</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2413,16 +2413,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>G117A</t>
+          <t>F45A</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>GLY</t>
+          <t>PHE</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2431,17 +2431,17 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>0.8</v>
+        <v>6.9</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>1flq</t>
+          <t>1fan</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">

</xml_diff>